<commit_message>
WS2812B Driver Bugfixes, ADC interface WIP
</commit_message>
<xml_diff>
--- a/documentation/ODESC_4p2 Pinout.xlsx
+++ b/documentation/ODESC_4p2 Pinout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\Github_Repos\Furuta-Pendulum\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B8B09E-0358-434C-9052-1C8ACBB044D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962FAE9B-B5DD-4966-807D-7039E4497A24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11475" yWindow="4365" windowWidth="24540" windowHeight="14325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43905" yWindow="3690" windowWidth="24540" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pinout" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="80">
   <si>
     <t>GPIO1</t>
   </si>
@@ -237,9 +237,6 @@
     <t>USB_DM D-</t>
   </si>
   <si>
-    <t>USB_DP D+</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -261,9 +258,6 @@
     <t>TIM1</t>
   </si>
   <si>
-    <t>not going to be used</t>
-  </si>
-  <si>
     <t>These are not connected to the MCU in the Odrive 3.5 schematic</t>
   </si>
   <si>
@@ -277,6 +271,12 @@
   </si>
   <si>
     <t>ENC_Z</t>
+  </si>
+  <si>
+    <t>USB_DP__LED_DO</t>
+  </si>
+  <si>
+    <t>used for sending info to WS2812B LED's</t>
   </si>
 </sst>
 </file>
@@ -609,14 +609,14 @@
   <dimension ref="C5:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.140625" customWidth="1"/>
+    <col min="6" max="6" width="27.85546875" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -625,13 +625,13 @@
         <v>4</v>
       </c>
       <c r="F5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" t="s">
         <v>67</v>
       </c>
-      <c r="G5" t="s">
-        <v>68</v>
-      </c>
       <c r="H5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.25">
@@ -645,7 +645,7 @@
         <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.25">
@@ -659,7 +659,7 @@
         <v>20</v>
       </c>
       <c r="G7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
@@ -673,13 +673,13 @@
         <v>21</v>
       </c>
       <c r="F8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
@@ -693,13 +693,13 @@
         <v>22</v>
       </c>
       <c r="F9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.25">
@@ -713,7 +713,7 @@
         <v>33</v>
       </c>
       <c r="G11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.25">
@@ -727,7 +727,7 @@
         <v>34</v>
       </c>
       <c r="G12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="3:8" x14ac:dyDescent="0.25">
@@ -741,7 +741,7 @@
         <v>35</v>
       </c>
       <c r="G13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.25">
@@ -755,7 +755,7 @@
         <v>36</v>
       </c>
       <c r="G14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.25">
@@ -772,7 +772,7 @@
         <v>63</v>
       </c>
       <c r="G15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
@@ -786,7 +786,7 @@
         <v>32</v>
       </c>
       <c r="G17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
@@ -800,7 +800,7 @@
         <v>31</v>
       </c>
       <c r="G18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
@@ -814,7 +814,7 @@
         <v>30</v>
       </c>
       <c r="G20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.25">
@@ -828,7 +828,7 @@
         <v>37</v>
       </c>
       <c r="G21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.25">
@@ -836,14 +836,14 @@
         <v>61</v>
       </c>
       <c r="D22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.25">
@@ -856,22 +856,19 @@
       <c r="E24" t="s">
         <v>58</v>
       </c>
-      <c r="F24" t="s">
-        <v>74</v>
-      </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>61</v>
       </c>
       <c r="D25" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="E25" t="s">
         <v>59</v>
       </c>
       <c r="F25" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.25">
@@ -882,7 +879,7 @@
         <v>7</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="3:9" x14ac:dyDescent="0.25">
@@ -916,7 +913,7 @@
         <v>47</v>
       </c>
       <c r="G35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="3:9" x14ac:dyDescent="0.25">
@@ -930,10 +927,10 @@
         <v>40</v>
       </c>
       <c r="G36" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I36" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="3:9" x14ac:dyDescent="0.25">
@@ -947,10 +944,10 @@
         <v>43</v>
       </c>
       <c r="G37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I37" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="3:9" x14ac:dyDescent="0.25">
@@ -964,10 +961,10 @@
         <v>41</v>
       </c>
       <c r="G38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" spans="3:9" x14ac:dyDescent="0.25">
@@ -981,10 +978,10 @@
         <v>44</v>
       </c>
       <c r="G39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="3:9" x14ac:dyDescent="0.25">
@@ -998,10 +995,10 @@
         <v>42</v>
       </c>
       <c r="G40" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="3:9" x14ac:dyDescent="0.25">
@@ -1015,10 +1012,10 @@
         <v>45</v>
       </c>
       <c r="G41" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I41" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="43" spans="3:9" x14ac:dyDescent="0.25">
@@ -1096,7 +1093,7 @@
         <v>48</v>
       </c>
       <c r="G50" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="3:7" x14ac:dyDescent="0.25">
@@ -1110,7 +1107,7 @@
         <v>49</v>
       </c>
       <c r="G51" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ADC Interface and NTC LUT
</commit_message>
<xml_diff>
--- a/documentation/ODESC_4p2 Pinout.xlsx
+++ b/documentation/ODESC_4p2 Pinout.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\Github_Repos\Furuta-Pendulum\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ross\Documents\GitHub\Furuta-Pendulum\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962FAE9B-B5DD-4966-807D-7039E4497A24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1BC507-3BA7-493D-8106-D57ADC8CA1AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43905" yWindow="3690" windowWidth="24540" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pinout" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="NXP15XH103F03RC " sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="95">
   <si>
     <t>GPIO1</t>
   </si>
@@ -277,6 +277,51 @@
   </si>
   <si>
     <t>used for sending info to WS2812B LED's</t>
+  </si>
+  <si>
+    <t>V_TEMP = AVCC / (R_NTC + R_BOT) * R_BOT</t>
+  </si>
+  <si>
+    <t>AVCC</t>
+  </si>
+  <si>
+    <t>R_BOT</t>
+  </si>
+  <si>
+    <t>RESOLUTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BITS </t>
+  </si>
+  <si>
+    <t>NTC P/N (assuming ODESC 4p2 uses same BOM as ODRIVE 3.5)</t>
+  </si>
+  <si>
+    <t>NXP15XH103F03RC</t>
+  </si>
+  <si>
+    <t>R_t2</t>
+  </si>
+  <si>
+    <t>t1</t>
+  </si>
+  <si>
+    <t>t2</t>
+  </si>
+  <si>
+    <t>B (25-100C)</t>
+  </si>
+  <si>
+    <t>B(1/t+1/t) = ln(Rt1/Rt2)</t>
+  </si>
+  <si>
+    <t>e^(B(1/t+1/t)) = Rt1/Rt2</t>
+  </si>
+  <si>
+    <t>Counts</t>
+  </si>
+  <si>
+    <t>CNTS = V_TEMP / AVCC * RESOLUTION</t>
   </si>
 </sst>
 </file>
@@ -318,7 +363,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -326,6 +371,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -341,6 +387,142 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>82550</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>241467</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95408</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2714B1FD-5D7F-FAD2-9DC7-FCCFEE883912}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5207000" y="152400"/>
+          <a:ext cx="3245017" cy="3073558"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>311151</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>565151</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>127142</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD9F0A3D-7FC6-72BF-4C4F-033E871B74FF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect r="35335"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10217151" y="304800"/>
+          <a:ext cx="4521200" cy="2768742"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>156</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>114386</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55E6C4FC-A36D-5EFA-C38B-5A49D7A1A255}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9315450" y="3238500"/>
+          <a:ext cx="3029106" cy="1663786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -608,19 +790,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C5:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="19.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.81640625" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.81640625" customWidth="1"/>
+    <col min="8" max="8" width="20.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:8" x14ac:dyDescent="0.35">
       <c r="E5" t="s">
         <v>4</v>
       </c>
@@ -634,7 +816,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
         <v>61</v>
       </c>
@@ -648,7 +830,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
         <v>61</v>
       </c>
@@ -662,7 +844,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
         <v>61</v>
       </c>
@@ -682,7 +864,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
         <v>61</v>
       </c>
@@ -702,7 +884,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
         <v>61</v>
       </c>
@@ -716,7 +898,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
         <v>61</v>
       </c>
@@ -730,7 +912,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
         <v>61</v>
       </c>
@@ -744,7 +926,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
         <v>61</v>
       </c>
@@ -758,7 +940,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C15" t="s">
         <v>61</v>
       </c>
@@ -775,7 +957,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C17" t="s">
         <v>61</v>
       </c>
@@ -789,7 +971,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C18" t="s">
         <v>61</v>
       </c>
@@ -803,7 +985,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
         <v>61</v>
       </c>
@@ -817,7 +999,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
         <v>61</v>
       </c>
@@ -831,7 +1013,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C22" t="s">
         <v>61</v>
       </c>
@@ -846,7 +1028,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C24" t="s">
         <v>61</v>
       </c>
@@ -857,7 +1039,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C25" t="s">
         <v>61</v>
       </c>
@@ -871,7 +1053,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C32" t="s">
         <v>61</v>
       </c>
@@ -882,7 +1064,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C33" t="s">
         <v>61</v>
       </c>
@@ -891,7 +1073,7 @@
       </c>
       <c r="F33" s="2"/>
     </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C34" t="s">
         <v>61</v>
       </c>
@@ -902,7 +1084,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C35" t="s">
         <v>61</v>
       </c>
@@ -916,7 +1098,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C36" t="s">
         <v>61</v>
       </c>
@@ -933,7 +1115,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C37" t="s">
         <v>61</v>
       </c>
@@ -950,7 +1132,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="38" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C38" t="s">
         <v>61</v>
       </c>
@@ -967,7 +1149,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C39" t="s">
         <v>61</v>
       </c>
@@ -984,7 +1166,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C40" t="s">
         <v>61</v>
       </c>
@@ -1001,7 +1183,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C41" t="s">
         <v>61</v>
       </c>
@@ -1018,7 +1200,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C43" t="s">
         <v>61</v>
       </c>
@@ -1029,7 +1211,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C44" t="s">
         <v>61</v>
       </c>
@@ -1040,7 +1222,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C46" t="s">
         <v>61</v>
       </c>
@@ -1054,7 +1236,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C47" t="s">
         <v>61</v>
       </c>
@@ -1068,7 +1250,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="48" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C48" t="s">
         <v>61</v>
       </c>
@@ -1082,7 +1264,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C50" t="s">
         <v>61</v>
       </c>
@@ -1096,7 +1278,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C51" t="s">
         <v>61</v>
       </c>
@@ -1122,12 +1304,781 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B7AA330-503A-49B9-80A7-BCFDDD29ED15}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:O79"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" customWidth="1"/>
+    <col min="7" max="7" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11">
+        <f>2^C10</f>
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13">
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="21" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="H21">
+        <v>274.14999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="E24" t="s">
+        <v>90</v>
+      </c>
+      <c r="F24">
+        <v>10000</v>
+      </c>
+      <c r="G24" t="s">
+        <v>87</v>
+      </c>
+      <c r="H24" t="s">
+        <v>88</v>
+      </c>
+      <c r="I24" t="s">
+        <v>89</v>
+      </c>
+      <c r="K24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="E25">
+        <v>3455</v>
+      </c>
+      <c r="F25">
+        <v>10000</v>
+      </c>
+      <c r="G25">
+        <f>F25/(EXP(E25*((1/($H$21+H25))-(1/($H$21+I25)))))</f>
+        <v>246828.50082754227</v>
+      </c>
+      <c r="H25">
+        <v>25</v>
+      </c>
+      <c r="I25">
+        <v>-40</v>
+      </c>
+      <c r="K25" s="3">
+        <f>$C$11/($C$13+G25)*$C$13</f>
+        <v>54.039423557411865</v>
+      </c>
+    </row>
+    <row r="26" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="E26">
+        <v>3455</v>
+      </c>
+      <c r="F26">
+        <v>10000</v>
+      </c>
+      <c r="G26">
+        <f t="shared" ref="G26:G41" si="0">F26/(EXP(E26*((1/($H$21+H26))-(1/($H$21+I26)))))</f>
+        <v>134872.75133045891</v>
+      </c>
+      <c r="H26">
+        <v>25</v>
+      </c>
+      <c r="I26">
+        <v>-30</v>
+      </c>
+      <c r="K26" s="3">
+        <f t="shared" ref="K26:K49" si="1">$C$11/($C$13+G26)*$C$13</f>
+        <v>97.82536621618496</v>
+      </c>
+    </row>
+    <row r="27" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="E27">
+        <v>3455</v>
+      </c>
+      <c r="F27">
+        <v>10000</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>77287.266178102058</v>
+      </c>
+      <c r="H27">
+        <v>25</v>
+      </c>
+      <c r="I27">
+        <v>-20</v>
+      </c>
+      <c r="K27" s="3">
+        <f t="shared" si="1"/>
+        <v>167.72873235490044</v>
+      </c>
+    </row>
+    <row r="28" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="E28">
+        <v>3455</v>
+      </c>
+      <c r="F28">
+        <v>10000</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>46195.607839338802</v>
+      </c>
+      <c r="H28">
+        <v>25</v>
+      </c>
+      <c r="I28">
+        <v>-10</v>
+      </c>
+      <c r="K28" s="3">
+        <f t="shared" si="1"/>
+        <v>273.09089816363326</v>
+      </c>
+    </row>
+    <row r="29" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="E29">
+        <v>3455</v>
+      </c>
+      <c r="F29">
+        <v>10000</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>28668.099185540497</v>
+      </c>
+      <c r="H29">
+        <v>25</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="K29" s="3">
+        <f t="shared" si="1"/>
+        <v>422.82151095532726</v>
+      </c>
+      <c r="O29" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="E30">
+        <v>3455</v>
+      </c>
+      <c r="F30">
+        <v>10000</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>18398.443489705667</v>
+      </c>
+      <c r="H30">
+        <v>25</v>
+      </c>
+      <c r="I30">
+        <v>10</v>
+      </c>
+      <c r="K30" s="3">
+        <f t="shared" si="1"/>
+        <v>622.93869172748441</v>
+      </c>
+    </row>
+    <row r="31" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="E31">
+        <v>3455</v>
+      </c>
+      <c r="F31">
+        <v>10000</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="0"/>
+        <v>12169.138637391874</v>
+      </c>
+      <c r="H31">
+        <v>25</v>
+      </c>
+      <c r="I31">
+        <v>20</v>
+      </c>
+      <c r="K31" s="3">
+        <f t="shared" si="1"/>
+        <v>873.79138016950094</v>
+      </c>
+      <c r="O31" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="E32">
+        <v>3455</v>
+      </c>
+      <c r="F32">
+        <v>10000</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="0"/>
+        <v>8270.7211357457963</v>
+      </c>
+      <c r="H32">
+        <v>25</v>
+      </c>
+      <c r="I32">
+        <v>30</v>
+      </c>
+      <c r="K32" s="3">
+        <f t="shared" si="1"/>
+        <v>1168.1899374657055</v>
+      </c>
+    </row>
+    <row r="33" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E33">
+        <v>3455</v>
+      </c>
+      <c r="F33">
+        <v>10000</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="0"/>
+        <v>5761.086466363975</v>
+      </c>
+      <c r="H33">
+        <v>25</v>
+      </c>
+      <c r="I33">
+        <v>40</v>
+      </c>
+      <c r="K33" s="3">
+        <f t="shared" si="1"/>
+        <v>1491.7416415985278</v>
+      </c>
+    </row>
+    <row r="34" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E34">
+        <v>3455</v>
+      </c>
+      <c r="F34">
+        <v>10000</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="0"/>
+        <v>4103.5023614527327</v>
+      </c>
+      <c r="H34">
+        <v>25</v>
+      </c>
+      <c r="I34">
+        <v>50</v>
+      </c>
+      <c r="K34" s="3">
+        <f t="shared" si="1"/>
+        <v>1825.7304907981015</v>
+      </c>
+    </row>
+    <row r="35" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E35">
+        <v>3455</v>
+      </c>
+      <c r="F35">
+        <v>10000</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="0"/>
+        <v>2982.8015272073576</v>
+      </c>
+      <c r="H35">
+        <v>25</v>
+      </c>
+      <c r="I35">
+        <v>60</v>
+      </c>
+      <c r="K35" s="3">
+        <f t="shared" si="1"/>
+        <v>2151.396943141714</v>
+      </c>
+    </row>
+    <row r="36" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E36">
+        <v>3455</v>
+      </c>
+      <c r="F36">
+        <v>10000</v>
+      </c>
+      <c r="G36">
+        <f>F36/(EXP(E36*((1/($H$21+H36))-(1/($H$21+I36)))))</f>
+        <v>2208.7400416494347</v>
+      </c>
+      <c r="H36">
+        <v>25</v>
+      </c>
+      <c r="I36">
+        <v>70</v>
+      </c>
+      <c r="K36" s="3">
+        <f t="shared" si="1"/>
+        <v>2453.7008277400541</v>
+      </c>
+    </row>
+    <row r="37" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E37">
+        <v>3455</v>
+      </c>
+      <c r="F37">
+        <v>10000</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="0"/>
+        <v>1663.5408398844263</v>
+      </c>
+      <c r="H37">
+        <v>25</v>
+      </c>
+      <c r="I37">
+        <v>80</v>
+      </c>
+      <c r="K37" s="3">
+        <f t="shared" si="1"/>
+        <v>2723.2172426961902</v>
+      </c>
+    </row>
+    <row r="38" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E38">
+        <v>3455</v>
+      </c>
+      <c r="F38">
+        <v>10000</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="0"/>
+        <v>1272.576478922656</v>
+      </c>
+      <c r="H38">
+        <v>25</v>
+      </c>
+      <c r="I38">
+        <v>90</v>
+      </c>
+      <c r="K38" s="3">
+        <f t="shared" si="1"/>
+        <v>2956.0577198229148</v>
+      </c>
+    </row>
+    <row r="39" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E39">
+        <v>3455</v>
+      </c>
+      <c r="F39">
+        <v>10000</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="0"/>
+        <v>987.53779188377439</v>
+      </c>
+      <c r="H39">
+        <v>25</v>
+      </c>
+      <c r="I39">
+        <v>100</v>
+      </c>
+      <c r="K39" s="3">
+        <f t="shared" si="1"/>
+        <v>3152.5786257994127</v>
+      </c>
+    </row>
+    <row r="40" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E40">
+        <v>3455</v>
+      </c>
+      <c r="F40">
+        <v>10000</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="0"/>
+        <v>776.52825670682455</v>
+      </c>
+      <c r="H40">
+        <v>25</v>
+      </c>
+      <c r="I40">
+        <v>110</v>
+      </c>
+      <c r="K40" s="3">
+        <f t="shared" si="1"/>
+        <v>3315.7626168202719</v>
+      </c>
+    </row>
+    <row r="41" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E41">
+        <v>3455</v>
+      </c>
+      <c r="F41">
+        <v>10000</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="0"/>
+        <v>618.09908233787269</v>
+      </c>
+      <c r="H41">
+        <v>25</v>
+      </c>
+      <c r="I41">
+        <v>120</v>
+      </c>
+      <c r="K41" s="3">
+        <f t="shared" si="1"/>
+        <v>3449.8361873826639</v>
+      </c>
+    </row>
+    <row r="42" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E42">
+        <v>3455</v>
+      </c>
+      <c r="F42">
+        <v>10000</v>
+      </c>
+      <c r="G42">
+        <f t="shared" ref="G42:G49" si="2">F42/(EXP(E42*((1/($H$21+H42))-(1/($H$21+I42)))))</f>
+        <v>497.58011069286306</v>
+      </c>
+      <c r="H42">
+        <v>25</v>
+      </c>
+      <c r="I42">
+        <v>130</v>
+      </c>
+      <c r="K42" s="3">
+        <f t="shared" si="1"/>
+        <v>3559.3192522629574</v>
+      </c>
+    </row>
+    <row r="43" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E43">
+        <v>3455</v>
+      </c>
+      <c r="F43">
+        <v>10000</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="2"/>
+        <v>404.77787403744497</v>
+      </c>
+      <c r="H43">
+        <v>25</v>
+      </c>
+      <c r="I43">
+        <v>140</v>
+      </c>
+      <c r="K43" s="3">
+        <f t="shared" si="1"/>
+        <v>3648.4778466001449</v>
+      </c>
+    </row>
+    <row r="44" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E44">
+        <v>3455</v>
+      </c>
+      <c r="F44">
+        <v>10000</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="2"/>
+        <v>332.50457016747879</v>
+      </c>
+      <c r="H44">
+        <v>25</v>
+      </c>
+      <c r="I44">
+        <v>150</v>
+      </c>
+      <c r="K44" s="3">
+        <f t="shared" si="1"/>
+        <v>3721.0689591442965</v>
+      </c>
+    </row>
+    <row r="45" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E45">
+        <v>3455</v>
+      </c>
+      <c r="F45">
+        <v>10000</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="2"/>
+        <v>275.62174559608877</v>
+      </c>
+      <c r="H45">
+        <v>25</v>
+      </c>
+      <c r="I45">
+        <v>160</v>
+      </c>
+      <c r="K45" s="3">
+        <f t="shared" si="1"/>
+        <v>3780.2656325848657</v>
+      </c>
+    </row>
+    <row r="46" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E46">
+        <v>3455</v>
+      </c>
+      <c r="F46">
+        <v>10000</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="2"/>
+        <v>230.40853154294933</v>
+      </c>
+      <c r="H46">
+        <v>25</v>
+      </c>
+      <c r="I46">
+        <v>170</v>
+      </c>
+      <c r="K46" s="3">
+        <f t="shared" si="1"/>
+        <v>3828.6787150076775</v>
+      </c>
+    </row>
+    <row r="47" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E47">
+        <v>3455</v>
+      </c>
+      <c r="F47">
+        <v>10000</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="2"/>
+        <v>194.13796420826</v>
+      </c>
+      <c r="H47">
+        <v>25</v>
+      </c>
+      <c r="I47">
+        <v>180</v>
+      </c>
+      <c r="K47" s="3">
+        <f t="shared" si="1"/>
+        <v>3868.4219508381043</v>
+      </c>
+    </row>
+    <row r="48" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E48">
+        <v>3455</v>
+      </c>
+      <c r="F48">
+        <v>10000</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="2"/>
+        <v>164.78881587076447</v>
+      </c>
+      <c r="H48">
+        <v>25</v>
+      </c>
+      <c r="I48">
+        <v>190</v>
+      </c>
+      <c r="K48" s="3">
+        <f t="shared" si="1"/>
+        <v>3901.1901499119167</v>
+      </c>
+    </row>
+    <row r="49" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="E49">
+        <v>3455</v>
+      </c>
+      <c r="F49">
+        <v>10000</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="2"/>
+        <v>140.84697882348229</v>
+      </c>
+      <c r="H49">
+        <v>25</v>
+      </c>
+      <c r="I49">
+        <v>200</v>
+      </c>
+      <c r="K49" s="3">
+        <f t="shared" si="1"/>
+        <v>3928.3351114386833</v>
+      </c>
+    </row>
+    <row r="55" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="F55">
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="56" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="F56">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="57" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="F57">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="58" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="F58">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="59" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="F59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="F60">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="F61">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="F62">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="63" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="F63">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="64" spans="5:11" x14ac:dyDescent="0.35">
+      <c r="F64">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="65" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F65">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F66">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="67" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F67">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="68" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F68">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="69" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F69">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="70" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F70">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="71" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F71">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="72" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F72">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="73" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F73">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="74" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F74">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="75" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F75">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="76" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F76">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="77" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F77">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="78" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F78">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="79" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F79">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ADC NTC's Interface, RGB LED control WIP, OLED display WIP
</commit_message>
<xml_diff>
--- a/documentation/ODESC_4p2 Pinout.xlsx
+++ b/documentation/ODESC_4p2 Pinout.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ross\Documents\GitHub\Furuta-Pendulum\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\Github_Repos\Furuta-Pendulum\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1BC507-3BA7-493D-8106-D57ADC8CA1AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C23F4E7-2B30-4E82-960B-7B576740C187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="42690" yWindow="3690" windowWidth="24540" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pinout" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="102">
   <si>
     <t>GPIO1</t>
   </si>
@@ -322,6 +322,27 @@
   </si>
   <si>
     <t>CNTS = V_TEMP / AVCC * RESOLUTION</t>
+  </si>
+  <si>
+    <t>encoder push button</t>
+  </si>
+  <si>
+    <t>repurposed as ssd1357 CS</t>
+  </si>
+  <si>
+    <t>repurposed as ssd1357 D#</t>
+  </si>
+  <si>
+    <t>Boot</t>
+  </si>
+  <si>
+    <t>timing/spare</t>
+  </si>
+  <si>
+    <t>repurposed as encoder rotary pos</t>
+  </si>
+  <si>
+    <t>soft button</t>
   </si>
 </sst>
 </file>
@@ -368,10 +389,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -788,21 +809,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C5:I51"/>
+  <dimension ref="C5:I48"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="19.81640625" customWidth="1"/>
-    <col min="5" max="5" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.81640625" customWidth="1"/>
-    <col min="8" max="8" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.85546875" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
         <v>4</v>
       </c>
@@ -816,7 +837,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>61</v>
       </c>
@@ -826,11 +847,14 @@
       <c r="E6" t="s">
         <v>19</v>
       </c>
+      <c r="F6" t="s">
+        <v>95</v>
+      </c>
       <c r="G6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>61</v>
       </c>
@@ -840,11 +864,14 @@
       <c r="E7" t="s">
         <v>20</v>
       </c>
+      <c r="F7" t="s">
+        <v>99</v>
+      </c>
       <c r="G7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>61</v>
       </c>
@@ -864,7 +891,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>61</v>
       </c>
@@ -884,7 +911,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>61</v>
       </c>
@@ -898,7 +925,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>61</v>
       </c>
@@ -912,7 +939,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>61</v>
       </c>
@@ -926,7 +953,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>61</v>
       </c>
@@ -940,7 +967,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>61</v>
       </c>
@@ -957,7 +984,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>61</v>
       </c>
@@ -971,7 +998,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>61</v>
       </c>
@@ -985,7 +1012,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>61</v>
       </c>
@@ -999,7 +1026,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>61</v>
       </c>
@@ -1013,7 +1040,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>61</v>
       </c>
@@ -1028,7 +1055,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>61</v>
       </c>
@@ -1038,8 +1065,11 @@
       <c r="E24" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="F24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>61</v>
       </c>
@@ -1053,27 +1083,69 @@
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" t="s">
+        <v>48</v>
+      </c>
+      <c r="F27" t="s">
+        <v>96</v>
+      </c>
+      <c r="G27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" t="s">
+        <v>49</v>
+      </c>
+      <c r="F28" t="s">
+        <v>97</v>
+      </c>
+      <c r="G28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>98</v>
+      </c>
+      <c r="F30" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>61</v>
       </c>
       <c r="D32" t="s">
         <v>7</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>61</v>
       </c>
       <c r="D33" t="s">
         <v>5</v>
       </c>
-      <c r="F33" s="2"/>
-    </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>61</v>
       </c>
@@ -1084,7 +1156,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>61</v>
       </c>
@@ -1098,7 +1170,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>61</v>
       </c>
@@ -1115,7 +1187,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>61</v>
       </c>
@@ -1132,7 +1204,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="38" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>61</v>
       </c>
@@ -1149,7 +1221,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>61</v>
       </c>
@@ -1166,7 +1238,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>61</v>
       </c>
@@ -1183,7 +1255,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
         <v>61</v>
       </c>
@@ -1200,7 +1272,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="43" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
         <v>61</v>
       </c>
@@ -1211,7 +1283,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
         <v>61</v>
       </c>
@@ -1222,7 +1294,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
         <v>61</v>
       </c>
@@ -1236,7 +1308,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
         <v>61</v>
       </c>
@@ -1250,7 +1322,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="48" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
         <v>61</v>
       </c>
@@ -1262,34 +1334,6 @@
       </c>
       <c r="F48" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C50" t="s">
-        <v>61</v>
-      </c>
-      <c r="D50" t="s">
-        <v>17</v>
-      </c>
-      <c r="E50" t="s">
-        <v>48</v>
-      </c>
-      <c r="G50" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C51" t="s">
-        <v>61</v>
-      </c>
-      <c r="D51" t="s">
-        <v>18</v>
-      </c>
-      <c r="E51" t="s">
-        <v>49</v>
-      </c>
-      <c r="G51" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1306,20 +1350,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B7AA330-503A-49B9-80A7-BCFDDD29ED15}">
   <dimension ref="B2:O79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.26953125" customWidth="1"/>
-    <col min="7" max="7" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.26953125" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>85</v>
       </c>
@@ -1327,17 +1371,17 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>84</v>
       </c>
@@ -1345,7 +1389,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>83</v>
       </c>
@@ -1354,7 +1398,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>81</v>
       </c>
@@ -1362,7 +1406,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>82</v>
       </c>
@@ -1370,12 +1414,12 @@
         <v>3300</v>
       </c>
     </row>
-    <row r="21" spans="5:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="5:15" x14ac:dyDescent="0.25">
       <c r="H21">
         <v>274.14999999999998</v>
       </c>
     </row>
-    <row r="24" spans="5:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
         <v>90</v>
       </c>
@@ -1395,7 +1439,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="5:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E25">
         <v>3455</v>
       </c>
@@ -1412,12 +1456,12 @@
       <c r="I25">
         <v>-40</v>
       </c>
-      <c r="K25" s="3">
+      <c r="K25" s="2">
         <f>$C$11/($C$13+G25)*$C$13</f>
         <v>54.039423557411865</v>
       </c>
     </row>
-    <row r="26" spans="5:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E26">
         <v>3455</v>
       </c>
@@ -1434,12 +1478,12 @@
       <c r="I26">
         <v>-30</v>
       </c>
-      <c r="K26" s="3">
+      <c r="K26" s="2">
         <f t="shared" ref="K26:K49" si="1">$C$11/($C$13+G26)*$C$13</f>
         <v>97.82536621618496</v>
       </c>
     </row>
-    <row r="27" spans="5:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E27">
         <v>3455</v>
       </c>
@@ -1456,12 +1500,12 @@
       <c r="I27">
         <v>-20</v>
       </c>
-      <c r="K27" s="3">
+      <c r="K27" s="2">
         <f t="shared" si="1"/>
         <v>167.72873235490044</v>
       </c>
     </row>
-    <row r="28" spans="5:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E28">
         <v>3455</v>
       </c>
@@ -1478,12 +1522,12 @@
       <c r="I28">
         <v>-10</v>
       </c>
-      <c r="K28" s="3">
+      <c r="K28" s="2">
         <f t="shared" si="1"/>
         <v>273.09089816363326</v>
       </c>
     </row>
-    <row r="29" spans="5:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E29">
         <v>3455</v>
       </c>
@@ -1500,7 +1544,7 @@
       <c r="I29">
         <v>0</v>
       </c>
-      <c r="K29" s="3">
+      <c r="K29" s="2">
         <f t="shared" si="1"/>
         <v>422.82151095532726</v>
       </c>
@@ -1508,7 +1552,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="5:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E30">
         <v>3455</v>
       </c>
@@ -1525,12 +1569,12 @@
       <c r="I30">
         <v>10</v>
       </c>
-      <c r="K30" s="3">
+      <c r="K30" s="2">
         <f t="shared" si="1"/>
         <v>622.93869172748441</v>
       </c>
     </row>
-    <row r="31" spans="5:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E31">
         <v>3455</v>
       </c>
@@ -1547,7 +1591,7 @@
       <c r="I31">
         <v>20</v>
       </c>
-      <c r="K31" s="3">
+      <c r="K31" s="2">
         <f t="shared" si="1"/>
         <v>873.79138016950094</v>
       </c>
@@ -1555,7 +1599,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="5:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="5:15" x14ac:dyDescent="0.25">
       <c r="E32">
         <v>3455</v>
       </c>
@@ -1572,12 +1616,12 @@
       <c r="I32">
         <v>30</v>
       </c>
-      <c r="K32" s="3">
+      <c r="K32" s="2">
         <f t="shared" si="1"/>
         <v>1168.1899374657055</v>
       </c>
     </row>
-    <row r="33" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E33">
         <v>3455</v>
       </c>
@@ -1594,12 +1638,12 @@
       <c r="I33">
         <v>40</v>
       </c>
-      <c r="K33" s="3">
+      <c r="K33" s="2">
         <f t="shared" si="1"/>
         <v>1491.7416415985278</v>
       </c>
     </row>
-    <row r="34" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E34">
         <v>3455</v>
       </c>
@@ -1616,12 +1660,12 @@
       <c r="I34">
         <v>50</v>
       </c>
-      <c r="K34" s="3">
+      <c r="K34" s="2">
         <f t="shared" si="1"/>
         <v>1825.7304907981015</v>
       </c>
     </row>
-    <row r="35" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E35">
         <v>3455</v>
       </c>
@@ -1638,12 +1682,12 @@
       <c r="I35">
         <v>60</v>
       </c>
-      <c r="K35" s="3">
+      <c r="K35" s="2">
         <f t="shared" si="1"/>
         <v>2151.396943141714</v>
       </c>
     </row>
-    <row r="36" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E36">
         <v>3455</v>
       </c>
@@ -1660,12 +1704,12 @@
       <c r="I36">
         <v>70</v>
       </c>
-      <c r="K36" s="3">
+      <c r="K36" s="2">
         <f t="shared" si="1"/>
         <v>2453.7008277400541</v>
       </c>
     </row>
-    <row r="37" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E37">
         <v>3455</v>
       </c>
@@ -1682,12 +1726,12 @@
       <c r="I37">
         <v>80</v>
       </c>
-      <c r="K37" s="3">
+      <c r="K37" s="2">
         <f t="shared" si="1"/>
         <v>2723.2172426961902</v>
       </c>
     </row>
-    <row r="38" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E38">
         <v>3455</v>
       </c>
@@ -1704,12 +1748,12 @@
       <c r="I38">
         <v>90</v>
       </c>
-      <c r="K38" s="3">
+      <c r="K38" s="2">
         <f t="shared" si="1"/>
         <v>2956.0577198229148</v>
       </c>
     </row>
-    <row r="39" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E39">
         <v>3455</v>
       </c>
@@ -1726,12 +1770,12 @@
       <c r="I39">
         <v>100</v>
       </c>
-      <c r="K39" s="3">
+      <c r="K39" s="2">
         <f t="shared" si="1"/>
         <v>3152.5786257994127</v>
       </c>
     </row>
-    <row r="40" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E40">
         <v>3455</v>
       </c>
@@ -1748,12 +1792,12 @@
       <c r="I40">
         <v>110</v>
       </c>
-      <c r="K40" s="3">
+      <c r="K40" s="2">
         <f t="shared" si="1"/>
         <v>3315.7626168202719</v>
       </c>
     </row>
-    <row r="41" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E41">
         <v>3455</v>
       </c>
@@ -1770,12 +1814,12 @@
       <c r="I41">
         <v>120</v>
       </c>
-      <c r="K41" s="3">
+      <c r="K41" s="2">
         <f t="shared" si="1"/>
         <v>3449.8361873826639</v>
       </c>
     </row>
-    <row r="42" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E42">
         <v>3455</v>
       </c>
@@ -1792,12 +1836,12 @@
       <c r="I42">
         <v>130</v>
       </c>
-      <c r="K42" s="3">
+      <c r="K42" s="2">
         <f t="shared" si="1"/>
         <v>3559.3192522629574</v>
       </c>
     </row>
-    <row r="43" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E43">
         <v>3455</v>
       </c>
@@ -1814,12 +1858,12 @@
       <c r="I43">
         <v>140</v>
       </c>
-      <c r="K43" s="3">
+      <c r="K43" s="2">
         <f t="shared" si="1"/>
         <v>3648.4778466001449</v>
       </c>
     </row>
-    <row r="44" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E44">
         <v>3455</v>
       </c>
@@ -1836,12 +1880,12 @@
       <c r="I44">
         <v>150</v>
       </c>
-      <c r="K44" s="3">
+      <c r="K44" s="2">
         <f t="shared" si="1"/>
         <v>3721.0689591442965</v>
       </c>
     </row>
-    <row r="45" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E45">
         <v>3455</v>
       </c>
@@ -1858,12 +1902,12 @@
       <c r="I45">
         <v>160</v>
       </c>
-      <c r="K45" s="3">
+      <c r="K45" s="2">
         <f t="shared" si="1"/>
         <v>3780.2656325848657</v>
       </c>
     </row>
-    <row r="46" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E46">
         <v>3455</v>
       </c>
@@ -1880,12 +1924,12 @@
       <c r="I46">
         <v>170</v>
       </c>
-      <c r="K46" s="3">
+      <c r="K46" s="2">
         <f t="shared" si="1"/>
         <v>3828.6787150076775</v>
       </c>
     </row>
-    <row r="47" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E47">
         <v>3455</v>
       </c>
@@ -1902,12 +1946,12 @@
       <c r="I47">
         <v>180</v>
       </c>
-      <c r="K47" s="3">
+      <c r="K47" s="2">
         <f t="shared" si="1"/>
         <v>3868.4219508381043</v>
       </c>
     </row>
-    <row r="48" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E48">
         <v>3455</v>
       </c>
@@ -1924,12 +1968,12 @@
       <c r="I48">
         <v>190</v>
       </c>
-      <c r="K48" s="3">
+      <c r="K48" s="2">
         <f t="shared" si="1"/>
         <v>3901.1901499119167</v>
       </c>
     </row>
-    <row r="49" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E49">
         <v>3455</v>
       </c>
@@ -1946,132 +1990,132 @@
       <c r="I49">
         <v>200</v>
       </c>
-      <c r="K49" s="3">
+      <c r="K49" s="2">
         <f t="shared" si="1"/>
         <v>3928.3351114386833</v>
       </c>
     </row>
-    <row r="55" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F55">
         <v>-40</v>
       </c>
     </row>
-    <row r="56" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="56" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F56">
         <v>-30</v>
       </c>
     </row>
-    <row r="57" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F57">
         <v>-20</v>
       </c>
     </row>
-    <row r="58" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F58">
         <v>-10</v>
       </c>
     </row>
-    <row r="59" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="59" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F59">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="60" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F60">
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="61" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F61">
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="62" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F62">
         <v>30</v>
       </c>
     </row>
-    <row r="63" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="63" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F63">
         <v>40</v>
       </c>
     </row>
-    <row r="64" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="64" spans="5:11" x14ac:dyDescent="0.25">
       <c r="F64">
         <v>50</v>
       </c>
     </row>
-    <row r="65" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F65">
         <v>60</v>
       </c>
     </row>
-    <row r="66" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F66">
         <v>70</v>
       </c>
     </row>
-    <row r="67" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F67">
         <v>80</v>
       </c>
     </row>
-    <row r="68" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F68">
         <v>90</v>
       </c>
     </row>
-    <row r="69" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F69">
         <v>100</v>
       </c>
     </row>
-    <row r="70" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F70">
         <v>110</v>
       </c>
     </row>
-    <row r="71" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F71">
         <v>120</v>
       </c>
     </row>
-    <row r="72" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F72">
         <v>130</v>
       </c>
     </row>
-    <row r="73" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="73" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F73">
         <v>140</v>
       </c>
     </row>
-    <row r="74" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F74">
         <v>150</v>
       </c>
     </row>
-    <row r="75" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="75" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F75">
         <v>160</v>
       </c>
     </row>
-    <row r="76" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F76">
         <v>170</v>
       </c>
     </row>
-    <row r="77" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F77">
         <v>180</v>
       </c>
     </row>
-    <row r="78" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F78">
         <v>190</v>
       </c>
     </row>
-    <row r="79" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F79">
         <v>200</v>
       </c>

</xml_diff>